<commit_message>
update to add zain
</commit_message>
<xml_diff>
--- a/player_ranking_data.xlsx
+++ b/player_ranking_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Timestamp</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Joimes</t>
+  </si>
+  <si>
+    <t>Zain</t>
   </si>
 </sst>
 </file>
@@ -1258,6 +1261,167 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>44550.538091504626</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="U6" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="V6" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="W6" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="X6" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AJ6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="AL6" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="AN6" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="AO6" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="AP6" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="AQ6" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="AR6" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="AS6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AT6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AU6" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="AV6" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="AW6" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="AX6" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="AY6" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="AZ6" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="BA6" s="5">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>